<commit_message>
close #140: Fix incorrect root node value in composicao.csv
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/composicao.xlsx
+++ b/input_data/data_ground_truth_01/composicao.xlsx
@@ -242,20 +242,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T934"/>
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="2" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -286,10 +286,10 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -311,11 +311,11 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>1</v>
+      <c r="A3" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -341,7 +341,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -367,7 +367,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -389,11 +389,11 @@
       <c r="T5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
-        <v>2</v>
+      <c r="A6" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -419,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -442,10 +442,10 @@
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -471,7 +471,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -493,12 +493,8 @@
       <c r="T9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>9</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -738,7 +734,7 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="4"/>
@@ -893,7 +889,7 @@
       <c r="T27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -915,8 +911,8 @@
       <c r="T28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -938,7 +934,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -960,7 +956,7 @@
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -982,7 +978,7 @@
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1004,7 +1000,7 @@
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1025,8 +1021,8 @@
       <c r="T33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1048,7 +1044,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1070,7 +1066,7 @@
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1092,7 +1088,7 @@
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1114,7 +1110,7 @@
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1136,7 +1132,7 @@
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1157,8 +1153,8 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1180,7 +1176,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1202,7 +1198,7 @@
     </row>
     <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
-      <c r="B42" s="7"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1224,7 +1220,7 @@
     </row>
     <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1246,7 +1242,7 @@
     </row>
     <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="7"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1267,8 +1263,8 @@
       <c r="T44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1290,7 +1286,7 @@
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="B46" s="5"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1312,7 +1308,7 @@
     </row>
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
-      <c r="B47" s="5"/>
+      <c r="B47" s="7"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1334,7 +1330,7 @@
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="B48" s="5"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1355,8 +1351,8 @@
       <c r="T48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="7"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1378,7 +1374,7 @@
     </row>
     <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
-      <c r="B50" s="7"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1400,7 +1396,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1422,7 +1418,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
-      <c r="B52" s="7"/>
+      <c r="B52" s="5"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1443,8 +1439,8 @@
       <c r="T52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1466,7 +1462,7 @@
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1488,7 +1484,7 @@
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
-      <c r="B55" s="5"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1510,7 +1506,7 @@
     </row>
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="B56" s="5"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1532,7 +1528,7 @@
     </row>
     <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
-      <c r="B57" s="5"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1575,8 +1571,8 @@
       <c r="T58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1598,7 +1594,7 @@
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="B60" s="7"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1619,7 +1615,7 @@
       <c r="T60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -1642,7 +1638,7 @@
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
+      <c r="B62" s="5"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -1664,7 +1660,7 @@
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
-      <c r="B63" s="5"/>
+      <c r="B63" s="7"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -1708,7 +1704,7 @@
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
+      <c r="B65" s="5"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -1730,7 +1726,7 @@
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
-      <c r="B66" s="5"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -1796,7 +1792,7 @@
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="B69" s="5"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -1818,7 +1814,7 @@
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="7"/>
-      <c r="B70" s="5"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -20824,28 +20820,7 @@
       <c r="S933" s="4"/>
       <c r="T933" s="4"/>
     </row>
-    <row r="934" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A934" s="7"/>
-      <c r="B934" s="7"/>
-      <c r="C934" s="4"/>
-      <c r="D934" s="4"/>
-      <c r="E934" s="4"/>
-      <c r="F934" s="4"/>
-      <c r="G934" s="4"/>
-      <c r="H934" s="4"/>
-      <c r="I934" s="4"/>
-      <c r="J934" s="4"/>
-      <c r="K934" s="4"/>
-      <c r="L934" s="4"/>
-      <c r="M934" s="4"/>
-      <c r="N934" s="4"/>
-      <c r="O934" s="4"/>
-      <c r="P934" s="4"/>
-      <c r="Q934" s="4"/>
-      <c r="R934" s="4"/>
-      <c r="S934" s="4"/>
-      <c r="T934" s="4"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>